<commit_message>
General debugging. Case 3 is passing and all tests are ok.
</commit_message>
<xml_diff>
--- a/tests/integration_cases/original/test_case2.xlsx
+++ b/tests/integration_cases/original/test_case2.xlsx
@@ -901,8 +901,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B1:H2993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2187" workbookViewId="0">
-      <selection activeCell="F2194" sqref="F2194"/>
+    <sheetView tabSelected="1" topLeftCell="A2964" workbookViewId="0">
+      <selection activeCell="F2985" sqref="F2985"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.3" x14ac:dyDescent="0.25"/>
@@ -25735,7 +25735,7 @@
         <v>8.0047999999999995</v>
       </c>
       <c r="F2985" s="24">
-        <v>41334</v>
+        <v>41699</v>
       </c>
     </row>
     <row r="2986" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>